<commit_message>
Reorganización del directorio Practica3_Kubernetes.
Reorganización del directorio Practica3_Kubernetes.
</commit_message>
<xml_diff>
--- a/Practicas/Practica 2/Practica MaaS/MapaEquiposDyD.xlsx
+++ b/Practicas/Practica 2/Practica MaaS/MapaEquiposDyD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Master\Segundo_Curso\servicios-smart-photos-team\Practicas\Practica 2\Practica MaaS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D818CD6-4514-4650-80D5-4CC4017C62D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6DF50B-4E44-4E69-827A-342458DEFF4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,13 +41,6 @@
 Host: 192.168.1.54</t>
   </si>
   <si>
-    <t>Z10: 
-Controladores K8s --&gt; Ready
-"merry-tetra", "pro-moose", "pumped-thrush"
-Controlador Juju --&gt; Ready
-Host: 192.168.1.50</t>
-  </si>
-  <si>
     <t>Z8: 
 Host: 192.168.1.59</t>
   </si>
@@ -57,11 +50,6 @@
 Host: 192.168.1.56</t>
   </si>
   <si>
-    <t>Z22: "Exact-cicada"
-Worker_8_Z22 --&gt; Ready
-Host: 192.168.1.57</t>
-  </si>
-  <si>
     <t>Z20: "sacred-pony"
 Worker_6_Z20 --&gt; Ready
 Host: 192.168.1.55</t>
@@ -72,11 +60,6 @@
 Host: 192.168.1.1</t>
   </si>
   <si>
-    <t>Z34: "Cosmic Cougar"
-Worker _2_Z34 --&gt; Ready
-Host:192.168.1.61</t>
-  </si>
-  <si>
     <t>Z36: "Still-dingo"
 Worker_1_Z36 --&gt; Ready
 Host: 192.168.1.51</t>
@@ -87,9 +70,28 @@
 Host: 192.168.1.58</t>
   </si>
   <si>
-    <t>Z42:  "brave-wolf"
+    <t>Z10: 
+Controladores K8s --&gt; Ready
+"merry-tetra" Juju Worker OK 
+"pro-moose" Juju Worker OK
+"pumped-thrush" Juju Worker OK
+Controlador Juju --&gt; Ready
+Host: 192.168.1.50</t>
+  </si>
+  <si>
+    <t>Z22: "Exact-cicada" Juju Worker OK
+Worker_8_Z22 --&gt; Ready
+Host: 192.168.1.57</t>
+  </si>
+  <si>
+    <t>Z34: "Cosmic Cougar" Juju Worker OK
+Worker _2_Z34 --&gt; Ready
+Host:192.168.1.61</t>
+  </si>
+  <si>
+    <t>Z42:  "brave-wolf" Juju Worker OK
 Worker_3_Z42--&gt; Ready
-192.168.1.62</t>
+Host 192.168.1.62</t>
   </si>
 </sst>
 </file>
@@ -703,7 +705,7 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,22 +740,22 @@
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="2:8" ht="93.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="118.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>5</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>0</v>
@@ -770,20 +772,20 @@
     </row>
     <row r="6" spans="2:8" ht="70.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>6</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>8</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>3</v>

</xml_diff>